<commit_message>
Added a comparison to add the closest child node to the bvh traversal stack and added its performance to the spreadsheet.
</commit_message>
<xml_diff>
--- a/BVH_Performance.xlsx
+++ b/BVH_Performance.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Projects\Radiance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A68F15D-7530-4BFA-A477-F336547BB356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53658AAD-DBAF-40FB-86D8-DE7B117087E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A5432B80-60C3-4BA9-AB2E-A1ED8FBAF94F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="unity.tri" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>SAH v1</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Orbit index</t>
+  </si>
+  <si>
+    <t>SAH v1 Closest child</t>
   </si>
 </sst>
 </file>
@@ -181,7 +184,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>unity.tri!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -204,7 +207,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$121</c:f>
+              <c:f>unity.tri!$A$2:$A$121</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="120"/>
@@ -573,7 +576,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$121</c:f>
+              <c:f>unity.tri!$B$2:$B$121</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="120"/>
@@ -952,7 +955,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>unity.tri!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -975,7 +978,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$121</c:f>
+              <c:f>unity.tri!$A$2:$A$121</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="120"/>
@@ -1344,7 +1347,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$121</c:f>
+              <c:f>unity.tri!$C$2:$C$121</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="120"/>
@@ -1715,6 +1718,777 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8108-4090-BCFD-2D6A4A741EE6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>unity.tri!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SAH v1 Closest child</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>unity.tri!$A$2:$A$121</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="120"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>unity.tri!$D$2:$D$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="120"/>
+                <c:pt idx="0">
+                  <c:v>20.155899999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>259.72399999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>252.66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>252.66800000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>244.268</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>232.41200000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>234.37700000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>241.50899999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>230.40100000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>225.864</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>222.364</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>216.083</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>212.85300000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>205.43700000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>200.214</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>141.92099999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>139.22900000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>131.46700000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>132.19399999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>146.74299999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>145.71600000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>145.26499999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>145.91800000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>159.55099999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>187.56</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>185.16499999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>184.471</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>187.11699999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>185.74600000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>183.03299999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>185.833</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>222.244</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>220.68899999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>207.19499999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>209.87700000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>199.16900000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>199.64599999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>194.029</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>192.56700000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>148.22300000000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>146.809</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>153.40799999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>174.17500000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>179.79</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>184.33</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>186.274</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>196.00800000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>200.69200000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>209.61600000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>220.69900000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>228.79599999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>235.221</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>239.05199999999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>253.18799999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>262.55399999999997</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>272.38400000000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>279.39600000000002</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>285.65600000000001</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>295.02600000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>290.23200000000003</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>260.77300000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>248.94399999999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>246.07499999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>234.315</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>233.56700000000001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>226.75</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>223.98500000000001</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>264.06200000000001</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>265.52600000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>273.37200000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>267.85300000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>283.47300000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>288.38</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>294.834</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>299.666</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>297.55700000000002</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>294.78100000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>312.30500000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>289.31200000000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>280.34800000000001</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>286.32900000000001</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>287.517</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>280.226</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>288.846</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>261.91399999999999</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>259.50299999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>250.423</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>178.75899999999999</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>184.52600000000001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>188.636</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>184.459</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>184.578</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>179.79900000000001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>168.59</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>168.95500000000001</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>170.124</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>167.94200000000001</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>166.32300000000001</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>160.43600000000001</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>158.63399999999999</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>154.535</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>157.36199999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>153.072</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>151.375</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>146.73500000000001</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>260.74099999999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>261.14100000000002</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>242.26400000000001</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>244.88800000000001</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>233.74100000000001</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>233.75299999999999</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>224.292</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>227.85400000000001</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>248.16200000000001</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>238.58099999999999</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>231.58199999999999</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>235.19200000000001</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>244.73599999999999</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>246.36099999999999</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>237.214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8108-4090-BCFD-2D6A4A741EE6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2612,16 +3386,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2966,18 +3740,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B414A2B-829D-47F4-B4A7-E3D786ED0D26}">
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2987,8 +3762,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2998,8 +3776,11 @@
       <c r="C2" s="1">
         <v>37.380000000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>20.155899999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3009,8 +3790,11 @@
       <c r="C3" s="1">
         <v>42.959499999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>259.72399999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3020,8 +3804,11 @@
       <c r="C4" s="1">
         <v>116.35599999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>252.66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3031,8 +3818,11 @@
       <c r="C5" s="1">
         <v>51.154400000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>252.66800000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3042,8 +3832,11 @@
       <c r="C6" s="1">
         <v>161.48500000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>244.268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3053,8 +3846,11 @@
       <c r="C7" s="1">
         <v>154.72399999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>232.41200000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3064,8 +3860,11 @@
       <c r="C8" s="1">
         <v>143.19499999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>234.37700000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3075,8 +3874,11 @@
       <c r="C9" s="1">
         <v>139.20400000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>241.50899999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3086,8 +3888,11 @@
       <c r="C10" s="1">
         <v>132.59899999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>230.40100000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3097,8 +3902,11 @@
       <c r="C11" s="1">
         <v>126.928</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>225.864</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3108,8 +3916,11 @@
       <c r="C12" s="1">
         <v>120.358</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>222.364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3119,8 +3930,11 @@
       <c r="C13" s="1">
         <v>114.372</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>216.083</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3130,8 +3944,11 @@
       <c r="C14" s="1">
         <v>107.29300000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>212.85300000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3141,8 +3958,11 @@
       <c r="C15" s="1">
         <v>113.33799999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>205.43700000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3152,8 +3972,11 @@
       <c r="C16" s="1">
         <v>111.045</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>200.214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3163,8 +3986,11 @@
       <c r="C17" s="1">
         <v>105.883</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>141.92099999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3174,8 +4000,11 @@
       <c r="C18" s="1">
         <v>112.654</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>139.22900000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3185,8 +4014,11 @@
       <c r="C19" s="1">
         <v>112.52800000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>131.46700000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3196,8 +4028,11 @@
       <c r="C20" s="1">
         <v>109.96299999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>132.19399999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3207,8 +4042,11 @@
       <c r="C21" s="1">
         <v>108.422</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>146.74299999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3218,8 +4056,11 @@
       <c r="C22" s="1">
         <v>105.887</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>145.71600000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3229,8 +4070,11 @@
       <c r="C23" s="1">
         <v>106.13800000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>145.26499999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -3240,8 +4084,11 @@
       <c r="C24" s="1">
         <v>104.774</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>145.91800000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3251,8 +4098,11 @@
       <c r="C25" s="1">
         <v>105.77500000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>159.55099999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -3262,8 +4112,11 @@
       <c r="C26" s="1">
         <v>105.35</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>187.56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -3273,8 +4126,11 @@
       <c r="C27" s="1">
         <v>107.855</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>185.16499999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -3284,8 +4140,11 @@
       <c r="C28" s="1">
         <v>109.381</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>184.471</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -3295,8 +4154,11 @@
       <c r="C29" s="1">
         <v>116.461</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>187.11699999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3306,8 +4168,11 @@
       <c r="C30" s="1">
         <v>122.242</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>185.74600000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -3317,8 +4182,11 @@
       <c r="C31" s="1">
         <v>124.03</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>183.03299999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -3328,8 +4196,11 @@
       <c r="C32" s="1">
         <v>127.456</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>185.833</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -3339,8 +4210,11 @@
       <c r="C33" s="1">
         <v>129.49799999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>222.244</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -3350,8 +4224,11 @@
       <c r="C34" s="1">
         <v>128.39599999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>220.68899999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -3361,8 +4238,11 @@
       <c r="C35" s="1">
         <v>126.74299999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <v>207.19499999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -3372,8 +4252,11 @@
       <c r="C36" s="1">
         <v>126.755</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>209.87700000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -3383,8 +4266,11 @@
       <c r="C37" s="1">
         <v>126.899</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37">
+        <v>199.16900000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3394,8 +4280,11 @@
       <c r="C38" s="1">
         <v>130.76</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>199.64599999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -3405,8 +4294,11 @@
       <c r="C39" s="1">
         <v>134.75299999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <v>194.029</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -3416,8 +4308,11 @@
       <c r="C40" s="1">
         <v>139.38999999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40">
+        <v>192.56700000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -3427,8 +4322,11 @@
       <c r="C41" s="1">
         <v>144.12899999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <v>148.22300000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -3438,8 +4336,11 @@
       <c r="C42" s="1">
         <v>152.85499999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42">
+        <v>146.809</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -3449,8 +4350,11 @@
       <c r="C43" s="1">
         <v>157.261</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43">
+        <v>153.40799999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3460,8 +4364,11 @@
       <c r="C44" s="1">
         <v>165.51300000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <v>174.17500000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -3471,8 +4378,11 @@
       <c r="C45" s="1">
         <v>173.125</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <v>179.79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -3482,8 +4392,11 @@
       <c r="C46" s="1">
         <v>163.798</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <v>184.33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -3493,8 +4406,11 @@
       <c r="C47" s="1">
         <v>176.65799999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <v>186.274</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3504,8 +4420,11 @@
       <c r="C48" s="1">
         <v>187.99299999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>196.00800000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -3515,8 +4434,11 @@
       <c r="C49" s="1">
         <v>181.976</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>200.69200000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3526,8 +4448,11 @@
       <c r="C50" s="1">
         <v>178.26</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>209.61600000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -3537,8 +4462,11 @@
       <c r="C51" s="1">
         <v>190.58</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <v>220.69900000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -3548,8 +4476,11 @@
       <c r="C52" s="1">
         <v>204.404</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>228.79599999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -3559,8 +4490,11 @@
       <c r="C53" s="1">
         <v>217.13399999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <v>235.221</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -3570,8 +4504,11 @@
       <c r="C54" s="1">
         <v>230.53399999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <v>239.05199999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -3581,8 +4518,11 @@
       <c r="C55" s="1">
         <v>245.71899999999999</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55">
+        <v>253.18799999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -3592,8 +4532,11 @@
       <c r="C56" s="1">
         <v>283.16199999999998</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56">
+        <v>262.55399999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -3603,8 +4546,11 @@
       <c r="C57" s="1">
         <v>285.82499999999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <v>272.38400000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -3614,8 +4560,11 @@
       <c r="C58" s="1">
         <v>296.12400000000002</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <v>279.39600000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -3625,8 +4574,11 @@
       <c r="C59" s="1">
         <v>309.60500000000002</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>285.65600000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -3636,8 +4588,11 @@
       <c r="C60" s="1">
         <v>317.81400000000002</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>295.02600000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -3647,8 +4602,11 @@
       <c r="C61" s="1">
         <v>315.50900000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>290.23200000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -3658,8 +4616,11 @@
       <c r="C62" s="1">
         <v>313.471</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <v>260.77300000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -3669,8 +4630,11 @@
       <c r="C63" s="1">
         <v>328.75200000000001</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <v>248.94399999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -3680,8 +4644,11 @@
       <c r="C64" s="1">
         <v>333.13299999999998</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <v>246.07499999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -3691,8 +4658,11 @@
       <c r="C65" s="1">
         <v>335.505</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <v>234.315</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -3702,8 +4672,11 @@
       <c r="C66" s="1">
         <v>230.739</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>233.56700000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -3713,8 +4686,11 @@
       <c r="C67" s="1">
         <v>225.893</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>226.75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -3724,8 +4700,11 @@
       <c r="C68" s="1">
         <v>222.60599999999999</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>223.98500000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -3735,8 +4714,11 @@
       <c r="C69" s="1">
         <v>219.642</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>264.06200000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -3746,8 +4728,11 @@
       <c r="C70" s="1">
         <v>214.126</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70">
+        <v>265.52600000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -3757,8 +4742,11 @@
       <c r="C71" s="1">
         <v>204.31100000000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>273.37200000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -3768,8 +4756,11 @@
       <c r="C72" s="1">
         <v>206.785</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72">
+        <v>267.85300000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -3779,8 +4770,11 @@
       <c r="C73" s="1">
         <v>186.61600000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>283.47300000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -3790,8 +4784,11 @@
       <c r="C74" s="1">
         <v>188.94</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>288.38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -3801,8 +4798,11 @@
       <c r="C75" s="1">
         <v>184.214</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>294.834</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -3812,8 +4812,11 @@
       <c r="C76" s="1">
         <v>183.36799999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>299.666</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -3823,8 +4826,11 @@
       <c r="C77" s="1">
         <v>179.06299999999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <v>297.55700000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -3834,8 +4840,11 @@
       <c r="C78" s="1">
         <v>176.84299999999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <v>294.78100000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -3845,8 +4854,11 @@
       <c r="C79" s="1">
         <v>178.27099999999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <v>312.30500000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -3856,8 +4868,11 @@
       <c r="C80" s="1">
         <v>175.61600000000001</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>289.31200000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -3867,8 +4882,11 @@
       <c r="C81" s="1">
         <v>187.55799999999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>280.34800000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -3878,8 +4896,11 @@
       <c r="C82" s="1">
         <v>213.375</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>286.32900000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -3889,8 +4910,11 @@
       <c r="C83" s="1">
         <v>218.136</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>287.517</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -3900,8 +4924,11 @@
       <c r="C84" s="1">
         <v>211.56</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>280.226</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -3911,8 +4938,11 @@
       <c r="C85" s="1">
         <v>224.35300000000001</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>288.846</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -3922,8 +4952,11 @@
       <c r="C86" s="1">
         <v>224.35400000000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>261.91399999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -3933,8 +4966,11 @@
       <c r="C87" s="1">
         <v>232.12299999999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>259.50299999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -3944,8 +4980,11 @@
       <c r="C88" s="1">
         <v>230.33500000000001</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>250.423</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -3955,8 +4994,11 @@
       <c r="C89" s="1">
         <v>236.291</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89">
+        <v>178.75899999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -3966,8 +5008,11 @@
       <c r="C90" s="1">
         <v>242.084</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <v>184.52600000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -3977,8 +5022,11 @@
       <c r="C91" s="1">
         <v>204.006</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <v>188.636</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -3988,8 +5036,11 @@
       <c r="C92" s="1">
         <v>194.727</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92">
+        <v>184.459</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -3999,8 +5050,11 @@
       <c r="C93" s="1">
         <v>194.084</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93">
+        <v>184.578</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -4010,8 +5064,11 @@
       <c r="C94" s="1">
         <v>250.309</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94">
+        <v>179.79900000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -4021,8 +5078,11 @@
       <c r="C95" s="1">
         <v>241.678</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <v>168.59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -4032,8 +5092,11 @@
       <c r="C96" s="1">
         <v>244.05099999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96">
+        <v>168.95500000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -4043,8 +5106,11 @@
       <c r="C97" s="1">
         <v>238.39699999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97">
+        <v>170.124</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -4054,8 +5120,11 @@
       <c r="C98" s="1">
         <v>226.31</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D98">
+        <v>167.94200000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -4065,8 +5134,11 @@
       <c r="C99" s="1">
         <v>223.322</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99">
+        <v>166.32300000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -4076,8 +5148,11 @@
       <c r="C100" s="1">
         <v>220.77699999999999</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100">
+        <v>160.43600000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -4087,8 +5162,11 @@
       <c r="C101" s="1">
         <v>210.78399999999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101">
+        <v>158.63399999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -4098,8 +5176,11 @@
       <c r="C102" s="1">
         <v>157.589</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102">
+        <v>154.535</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -4109,8 +5190,11 @@
       <c r="C103" s="1">
         <v>149.327</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103">
+        <v>157.36199999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -4120,8 +5204,11 @@
       <c r="C104" s="1">
         <v>143.30799999999999</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104">
+        <v>153.072</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -4131,8 +5218,11 @@
       <c r="C105" s="1">
         <v>135.90799999999999</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D105">
+        <v>151.375</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -4142,8 +5232,11 @@
       <c r="C106" s="1">
         <v>132.07300000000001</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106">
+        <v>146.73500000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -4153,8 +5246,11 @@
       <c r="C107" s="1">
         <v>127.86499999999999</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107">
+        <v>260.74099999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -4164,8 +5260,11 @@
       <c r="C108" s="1">
         <v>167.471</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108">
+        <v>261.14100000000002</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -4175,8 +5274,11 @@
       <c r="C109" s="1">
         <v>162.245</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D109">
+        <v>242.26400000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -4186,8 +5288,11 @@
       <c r="C110" s="1">
         <v>155.61000000000001</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D110">
+        <v>244.88800000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -4197,8 +5302,11 @@
       <c r="C111" s="1">
         <v>151.63200000000001</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D111">
+        <v>233.74100000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -4208,8 +5316,11 @@
       <c r="C112" s="1">
         <v>146.446</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D112">
+        <v>233.75299999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -4219,8 +5330,11 @@
       <c r="C113" s="1">
         <v>142.172</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113">
+        <v>224.292</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -4230,8 +5344,11 @@
       <c r="C114" s="1">
         <v>139.459</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114">
+        <v>227.85400000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -4241,8 +5358,11 @@
       <c r="C115" s="1">
         <v>133.315</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115">
+        <v>248.16200000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -4252,8 +5372,11 @@
       <c r="C116" s="1">
         <v>128.18100000000001</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D116">
+        <v>238.58099999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -4263,8 +5386,11 @@
       <c r="C117" s="1">
         <v>148.53800000000001</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D117">
+        <v>231.58199999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -4274,8 +5400,11 @@
       <c r="C118" s="1">
         <v>143.09200000000001</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118">
+        <v>235.19200000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -4285,8 +5414,11 @@
       <c r="C119" s="1">
         <v>133.71700000000001</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D119">
+        <v>244.73599999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -4296,8 +5428,11 @@
       <c r="C120" s="1">
         <v>132.34399999999999</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D120">
+        <v>246.36099999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -4306,6 +5441,9 @@
       </c>
       <c r="C121" s="1">
         <v>127.39100000000001</v>
+      </c>
+      <c r="D121">
+        <v>237.214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>